<commit_message>
add dates info and populate map with dates
</commit_message>
<xml_diff>
--- a/data/dates/dates_9_5_16.xlsx
+++ b/data/dates/dates_9_5_16.xlsx
@@ -16,7 +16,7 @@
     <sheet name="region_key" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$E$8:$E$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$F$8:$F$19</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="132">
   <si>
     <t>Southeast</t>
   </si>
@@ -156,9 +156,6 @@
     <t>San Francisco</t>
   </si>
   <si>
-    <t>Portlant</t>
-  </si>
-  <si>
     <t>Seattle</t>
   </si>
   <si>
@@ -223,13 +220,220 @@
   </si>
   <si>
     <t>post_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>NYC</t>
+  </si>
+  <si>
+    <t>WAS</t>
+  </si>
+  <si>
+    <t>PHL</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>NOL</t>
+  </si>
+  <si>
+    <t>NSH</t>
+  </si>
+  <si>
+    <t>ORL</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>AUS</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>PHX</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>REN</t>
+  </si>
+  <si>
+    <t>LAV</t>
+  </si>
+  <si>
+    <t>LAS</t>
+  </si>
+  <si>
+    <t>SFO</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>PDX</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>SDG</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>CLV</t>
+  </si>
+  <si>
+    <t>city_id</t>
+  </si>
+  <si>
+    <t>MIA4268742692NFHB</t>
+  </si>
+  <si>
+    <t>MIA4269442697DHCU</t>
+  </si>
+  <si>
+    <t>MIA4271642723EHAX</t>
+  </si>
+  <si>
+    <t>MIA4280642811JYQN</t>
+  </si>
+  <si>
+    <t>MIA4282842833HZGV</t>
+  </si>
+  <si>
+    <t>DAL4264542648NAHB</t>
+  </si>
+  <si>
+    <t>DAL4265242657IUFI</t>
+  </si>
+  <si>
+    <t>DAL4267342678ITVG</t>
+  </si>
+  <si>
+    <t>DAL4268042685OIEO</t>
+  </si>
+  <si>
+    <t>DAL4268742691CROK</t>
+  </si>
+  <si>
+    <t>DAL4270142704QUNS</t>
+  </si>
+  <si>
+    <t>DAL4270842712PSVA</t>
+  </si>
+  <si>
+    <t>DAL4271542720KVNS</t>
+  </si>
+  <si>
+    <t>DAL4272242727EZEN</t>
+  </si>
+  <si>
+    <t>DAL4287642880CYKD</t>
+  </si>
+  <si>
+    <t>DAL4291142915SDZI</t>
+  </si>
+  <si>
+    <t>DAL4298842993RUTI</t>
+  </si>
+  <si>
+    <t>DAL4299542999AUTT</t>
+  </si>
+  <si>
+    <t>REN4268042683RLXS</t>
+  </si>
+  <si>
+    <t>REN4269442697OABM</t>
+  </si>
+  <si>
+    <t>REN4270942712YDTF</t>
+  </si>
+  <si>
+    <t>REN4271642719VHDG</t>
+  </si>
+  <si>
+    <t>REN4273842741WHLU</t>
+  </si>
+  <si>
+    <t>REN4283442837BEUO</t>
+  </si>
+  <si>
+    <t>REN4285542857LBLI</t>
+  </si>
+  <si>
+    <t>REN4286942872TLAI</t>
+  </si>
+  <si>
+    <t>REN4287742880IDUB</t>
+  </si>
+  <si>
+    <t>REN4288342888IWGB</t>
+  </si>
+  <si>
+    <t>REN4289042894YVNK</t>
+  </si>
+  <si>
+    <t>REN4291142916LXRL</t>
+  </si>
+  <si>
+    <t>REN4291842921PPJE</t>
+  </si>
+  <si>
+    <t>REN4293242935JPQG</t>
+  </si>
+  <si>
+    <t>REN4296042964HHRQ</t>
+  </si>
+  <si>
+    <t>REN4296742971CNZL</t>
+  </si>
+  <si>
+    <t>REN4297442978TQAY</t>
+  </si>
+  <si>
+    <t>REN4298242985BDEV</t>
+  </si>
+  <si>
+    <t>REN4307243075TJOW</t>
+  </si>
+  <si>
+    <t>REN4308643090XKIS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -237,19 +441,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -279,21 +485,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,18 +774,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -596,25 +798,28 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" t="s">
         <v>62</v>
       </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -627,25 +832,23 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="1">
         <v>42687</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>42692</v>
       </c>
-      <c r="G2" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J2" t="str">
-        <f>CONCATENATE(B2,LEFT(C2,3))</f>
-        <v>SEMia</v>
-      </c>
-      <c r="K2">
-        <f>MONTH(F2)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H2" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -658,21 +861,23 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="1">
         <v>42694</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>42697</v>
       </c>
-      <c r="G3" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J39" si="0">CONCATENATE(B3,LEFT(C3,3))</f>
-        <v>SEMia</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H3" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -685,21 +890,26 @@
       <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="1">
         <v>42716</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>42723</v>
       </c>
-      <c r="G4" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J4" t="str">
-        <f t="shared" si="0"/>
-        <v>SEMia</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H4" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -712,21 +922,23 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="1">
         <v>42806</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>42811</v>
       </c>
-      <c r="G5" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v>SEMia</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H5" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -739,21 +951,23 @@
       <c r="D6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="1">
         <v>42828</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>42833</v>
       </c>
-      <c r="G6" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>SEMia</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H6" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -766,21 +980,23 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="1">
         <v>42645</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>42648</v>
       </c>
-      <c r="G7" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H7" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -793,21 +1009,23 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="1">
         <v>42652</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>42657</v>
       </c>
-      <c r="G8" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H8" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -820,21 +1038,23 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="1">
         <v>42673</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>42678</v>
       </c>
-      <c r="G9" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H9" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -847,24 +1067,26 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="1">
         <v>42680</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>42685</v>
       </c>
-      <c r="G10" s="1">
-        <v>42618</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="H10" s="1">
+        <v>42618</v>
+      </c>
+      <c r="J10" t="s">
         <v>13</v>
       </c>
-      <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -877,21 +1099,23 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="1">
         <v>42687</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>42691</v>
       </c>
-      <c r="G11" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J11" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H11" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -904,21 +1128,23 @@
       <c r="D12" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="1">
         <v>42701</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>42704</v>
       </c>
-      <c r="G12" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J12" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H12" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -931,21 +1157,23 @@
       <c r="D13" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="1">
         <v>42708</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>42712</v>
       </c>
-      <c r="G13" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J13" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H13" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -958,21 +1186,23 @@
       <c r="D14" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" s="1">
         <v>42715</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>42720</v>
       </c>
-      <c r="G14" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H14" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -985,21 +1215,23 @@
       <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="1">
         <v>42722</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>42727</v>
       </c>
-      <c r="G15" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J15" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H15" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1012,21 +1244,23 @@
       <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="1">
         <v>42876</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>42880</v>
       </c>
-      <c r="G16" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J16" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H16" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1039,21 +1273,23 @@
       <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="1">
         <v>42911</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>42915</v>
       </c>
-      <c r="G17" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J17" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H17" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1066,21 +1302,23 @@
       <c r="D18" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="1">
         <v>42988</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>42993</v>
       </c>
-      <c r="G18" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J18" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H18" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1093,21 +1331,23 @@
       <c r="D19" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="1">
         <v>42995</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>42999</v>
       </c>
-      <c r="G19" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J19" t="str">
-        <f t="shared" si="0"/>
-        <v>SWDal</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H19" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1120,21 +1360,23 @@
       <c r="D20" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="2">
         <v>42680</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>42683</v>
       </c>
-      <c r="G20" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J20" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H20" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1147,21 +1389,23 @@
       <c r="D21" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="1">
         <v>42694</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>42697</v>
       </c>
-      <c r="G21" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J21" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H21" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K21" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1174,21 +1418,23 @@
       <c r="D22" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" t="s">
+        <v>82</v>
+      </c>
+      <c r="F22" s="1">
         <v>42709</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>42712</v>
       </c>
-      <c r="G22" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J22" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H22" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K22" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -1201,21 +1447,23 @@
       <c r="D23" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F23" s="1">
         <v>42716</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>42719</v>
       </c>
-      <c r="G23" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J23" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H23" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1228,21 +1476,23 @@
       <c r="D24" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="1">
         <v>42738</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>42741</v>
       </c>
-      <c r="G24" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J24" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H24" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -1255,21 +1505,23 @@
       <c r="D25" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="1">
         <v>42834</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>42837</v>
       </c>
-      <c r="G25" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J25" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H25" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1282,21 +1534,23 @@
       <c r="D26" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="1">
         <v>42855</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>42857</v>
       </c>
-      <c r="G26" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J26" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H26" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -1309,21 +1563,23 @@
       <c r="D27" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="1">
         <v>42869</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>42872</v>
       </c>
-      <c r="G27" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J27" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H27" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K27" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -1336,21 +1592,23 @@
       <c r="D28" t="s">
         <v>18</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="1">
         <v>42877</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>42880</v>
       </c>
-      <c r="G28" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J28" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H28" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K28" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1363,24 +1621,26 @@
       <c r="D29" t="s">
         <v>18</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F29" s="1">
         <v>42883</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>42888</v>
       </c>
-      <c r="G29" s="1">
-        <v>42618</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="H29" s="1">
+        <v>42618</v>
+      </c>
+      <c r="J29" t="s">
         <v>13</v>
       </c>
-      <c r="J29" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -1393,21 +1653,23 @@
       <c r="D30" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="1">
         <v>42890</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>42894</v>
       </c>
-      <c r="G30" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J30" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H30" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -1420,21 +1682,23 @@
       <c r="D31" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="1">
         <v>42911</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>42916</v>
       </c>
-      <c r="G31" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J31" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H31" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1447,24 +1711,26 @@
       <c r="D32" t="s">
         <v>18</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="1">
         <v>42918</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>42921</v>
       </c>
-      <c r="G32" s="1">
-        <v>42618</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="H32" s="1">
+        <v>42618</v>
+      </c>
+      <c r="J32" t="s">
         <v>13</v>
       </c>
-      <c r="J32" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>19</v>
       </c>
@@ -1477,21 +1743,23 @@
       <c r="D33" t="s">
         <v>18</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="1">
         <v>42932</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="1">
         <v>42935</v>
       </c>
-      <c r="G33" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J33" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H33" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>19</v>
       </c>
@@ -1504,21 +1772,23 @@
       <c r="D34" t="s">
         <v>18</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="1">
         <v>42960</v>
       </c>
-      <c r="F34" s="1">
+      <c r="G34" s="1">
         <v>42964</v>
       </c>
-      <c r="G34" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J34" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H34" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>19</v>
       </c>
@@ -1531,21 +1801,23 @@
       <c r="D35" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" s="1">
         <v>42967</v>
       </c>
-      <c r="F35" s="1">
+      <c r="G35" s="1">
         <v>42971</v>
       </c>
-      <c r="G35" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J35" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H35" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -1558,21 +1830,23 @@
       <c r="D36" t="s">
         <v>18</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" t="s">
+        <v>82</v>
+      </c>
+      <c r="F36" s="1">
         <v>42974</v>
       </c>
-      <c r="F36" s="1">
+      <c r="G36" s="1">
         <v>42978</v>
       </c>
-      <c r="G36" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J36" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H36" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K36" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>19</v>
       </c>
@@ -1585,24 +1859,26 @@
       <c r="D37" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="1">
         <v>42982</v>
       </c>
-      <c r="F37" s="1">
+      <c r="G37" s="1">
         <v>42985</v>
       </c>
-      <c r="G37" s="1">
-        <v>42618</v>
-      </c>
-      <c r="I37" t="s">
+      <c r="H37" s="1">
+        <v>42618</v>
+      </c>
+      <c r="J37" t="s">
         <v>13</v>
       </c>
-      <c r="J37" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -1615,21 +1891,23 @@
       <c r="D38" t="s">
         <v>18</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="1">
         <v>43072</v>
       </c>
-      <c r="F38" s="1">
+      <c r="G38" s="1">
         <v>43075</v>
       </c>
-      <c r="G38" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J38" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H38" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K38" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -1642,304 +1920,500 @@
       <c r="D39" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" s="1">
         <v>43086</v>
       </c>
-      <c r="F39" s="1">
+      <c r="G39" s="1">
         <v>43090</v>
       </c>
-      <c r="G39" s="1">
-        <v>42618</v>
-      </c>
-      <c r="J39" t="str">
-        <f t="shared" si="0"/>
-        <v>WCRen</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G40" s="1"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G41" s="1"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G42" s="1"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G43" s="1"/>
+      <c r="H39" s="1">
+        <v>42618</v>
+      </c>
+      <c r="K39" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H43" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="E8:E19"/>
+  <autoFilter ref="F8:F19"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="C4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="C5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D9" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="E9" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="C7" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="D13" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="C9" s="4" t="s">
+      <c r="E13" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="E14" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="C12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="E17" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="C18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="C15" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="C16" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="C17" s="4" t="s">
+      <c r="E18" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="C19" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
+      <c r="D19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="C21" s="4" t="s">
+      <c r="E20" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="C22" s="3" t="s">
+      <c r="E22" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="C23" s="4" t="s">
+      <c r="D24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-      <c r="C24" s="3" t="s">
+      <c r="D25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D26" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-      <c r="C25" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" t="s">
-        <v>49</v>
+      <c r="E26" s="3" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E26">
+    <sortCondition ref="A2:A26"/>
+    <sortCondition ref="C2:C26"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>